<commit_message>
Korrekturen markup index und key values
</commit_message>
<xml_diff>
--- a/data/xlsx/Baernreither_Index_2023.xlsx
+++ b/data/xlsx/Baernreither_Index_2023.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christofaichner/Documents/GitHub/baernreither-data/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christofaichner/Documents/GitHub/baernreither-data/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12220"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13720"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -212,9 +212,6 @@
     <t>Proportionalwahlrecht</t>
   </si>
   <si>
-    <t>Taaffe'sche Wahlreform</t>
-  </si>
-  <si>
     <t>Wahlkampf</t>
   </si>
   <si>
@@ -291,6 +288,9 @@
   </si>
   <si>
     <t>Paragraph 14 des Gesetzes vom 21. Dezember 1867</t>
+  </si>
+  <si>
+    <t>Taaffesche Wahlreform</t>
   </si>
 </sst>
 </file>
@@ -676,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -697,25 +697,25 @@
     </row>
     <row r="3" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>83</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>13</v>
@@ -723,7 +723,7 @@
     </row>
     <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>14</v>
@@ -731,7 +731,7 @@
     </row>
     <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>15</v>
@@ -739,7 +739,7 @@
     </row>
     <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>36</v>
@@ -747,26 +747,26 @@
     </row>
     <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.2">
@@ -776,7 +776,7 @@
     </row>
     <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>16</v>
@@ -784,7 +784,7 @@
     </row>
     <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>17</v>
@@ -797,7 +797,7 @@
     </row>
     <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>18</v>
@@ -805,10 +805,10 @@
     </row>
     <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.2">
@@ -818,7 +818,7 @@
     </row>
     <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>19</v>
@@ -849,7 +849,7 @@
     </row>
     <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>21</v>
@@ -857,7 +857,7 @@
     </row>
     <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>22</v>
@@ -865,7 +865,7 @@
     </row>
     <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>23</v>
@@ -873,7 +873,7 @@
     </row>
     <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>24</v>
@@ -881,7 +881,7 @@
     </row>
     <row r="29" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>25</v>
@@ -889,7 +889,7 @@
     </row>
     <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>26</v>
@@ -897,7 +897,7 @@
     </row>
     <row r="31" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>27</v>
@@ -905,7 +905,7 @@
     </row>
     <row r="32" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>28</v>
@@ -913,7 +913,7 @@
     </row>
     <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>29</v>
@@ -921,7 +921,7 @@
     </row>
     <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>30</v>
@@ -929,7 +929,7 @@
     </row>
     <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>31</v>
@@ -937,7 +937,7 @@
     </row>
     <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>17</v>
@@ -945,7 +945,7 @@
     </row>
     <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>32</v>
@@ -966,7 +966,7 @@
         <v>7</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15" x14ac:dyDescent="0.2">
@@ -992,7 +992,7 @@
     </row>
     <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>35</v>
@@ -1000,7 +1000,7 @@
     </row>
     <row r="45" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>36</v>
@@ -1008,7 +1008,7 @@
     </row>
     <row r="46" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>37</v>
@@ -1016,7 +1016,7 @@
     </row>
     <row r="47" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>38</v>
@@ -1024,7 +1024,7 @@
     </row>
     <row r="48" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>39</v>
@@ -1032,7 +1032,7 @@
     </row>
     <row r="49" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>40</v>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="50" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>41</v>
@@ -1048,7 +1048,7 @@
     </row>
     <row r="51" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>42</v>
@@ -1056,7 +1056,7 @@
     </row>
     <row r="52" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>43</v>
@@ -1064,7 +1064,7 @@
     </row>
     <row r="53" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>44</v>
@@ -1072,7 +1072,7 @@
     </row>
     <row r="54" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>45</v>
@@ -1090,7 +1090,7 @@
     </row>
     <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>40</v>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="58" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>46</v>
@@ -1106,7 +1106,7 @@
     </row>
     <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>47</v>
@@ -1114,7 +1114,7 @@
     </row>
     <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>21</v>
@@ -1122,7 +1122,7 @@
     </row>
     <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>48</v>
@@ -1130,7 +1130,7 @@
     </row>
     <row r="62" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>49</v>
@@ -1138,12 +1138,12 @@
     </row>
     <row r="63" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>50</v>
@@ -1151,7 +1151,7 @@
     </row>
     <row r="65" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>51</v>
@@ -1231,7 +1231,7 @@
         <v>46</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="15" x14ac:dyDescent="0.2">
@@ -1239,7 +1239,7 @@
         <v>46</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="15" x14ac:dyDescent="0.2">
@@ -1247,7 +1247,7 @@
         <v>46</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="15" x14ac:dyDescent="0.2">
@@ -1255,12 +1255,12 @@
         <v>46</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Korrekturen key values und allgemeine Korrekturen
</commit_message>
<xml_diff>
--- a/data/xlsx/Baernreither_Index_2023.xlsx
+++ b/data/xlsx/Baernreither_Index_2023.xlsx
@@ -77,9 +77,6 @@
     <t>Gymnasialzeit</t>
   </si>
   <si>
-    <t>Studien England 1883/84</t>
-  </si>
-  <si>
     <t>Zollbündnis mit Österreich-Ungarn</t>
   </si>
   <si>
@@ -194,9 +191,6 @@
     <t>Arbeiterkurie</t>
   </si>
   <si>
-    <t xml:space="preserve">Badeni'sche Wahlreform </t>
-  </si>
-  <si>
     <t>Kurie Allgemeine Wählerklasse</t>
   </si>
   <si>
@@ -291,6 +285,12 @@
   </si>
   <si>
     <t>Taaffesche Wahlreform</t>
+  </si>
+  <si>
+    <t>Studien England</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Badenische Wahlreform </t>
   </si>
 </sst>
 </file>
@@ -676,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -697,25 +697,25 @@
     </row>
     <row r="3" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>13</v>
@@ -723,7 +723,7 @@
     </row>
     <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>14</v>
@@ -731,42 +731,42 @@
     </row>
     <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.2">
@@ -776,18 +776,18 @@
     </row>
     <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.2">
@@ -797,18 +797,18 @@
     </row>
     <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.2">
@@ -818,10 +818,10 @@
     </row>
     <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.2">
@@ -844,111 +844,111 @@
         <v>5</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15" x14ac:dyDescent="0.2">
@@ -966,7 +966,7 @@
         <v>7</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15" x14ac:dyDescent="0.2">
@@ -974,7 +974,7 @@
         <v>7</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15" x14ac:dyDescent="0.2">
@@ -982,7 +982,7 @@
         <v>7</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15" x14ac:dyDescent="0.2">
@@ -992,90 +992,90 @@
     </row>
     <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15" x14ac:dyDescent="0.2">
@@ -1090,177 +1090,177 @@
     </row>
     <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Korrekturen orgname und persname, kontrolle index
</commit_message>
<xml_diff>
--- a/data/xlsx/Baernreither_Index_2023.xlsx
+++ b/data/xlsx/Baernreither_Index_2023.xlsx
@@ -116,9 +116,6 @@
     <t>Verhältnis zueinander</t>
   </si>
   <si>
-    <t>wirtschaftliche Trennung</t>
-  </si>
-  <si>
     <t>Zoll- und Handelsbündnis</t>
   </si>
   <si>
@@ -291,6 +288,9 @@
   </si>
   <si>
     <t xml:space="preserve">Badenische Wahlreform </t>
+  </si>
+  <si>
+    <t>Wirtschaftliche Trennung</t>
   </si>
 </sst>
 </file>
@@ -676,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -697,25 +697,25 @@
     </row>
     <row r="3" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>13</v>
@@ -723,7 +723,7 @@
     </row>
     <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>14</v>
@@ -731,42 +731,42 @@
     </row>
     <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.2">
@@ -776,7 +776,7 @@
     </row>
     <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>15</v>
@@ -784,7 +784,7 @@
     </row>
     <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>16</v>
@@ -797,7 +797,7 @@
     </row>
     <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>17</v>
@@ -805,10 +805,10 @@
     </row>
     <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.2">
@@ -818,7 +818,7 @@
     </row>
     <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>18</v>
@@ -849,7 +849,7 @@
     </row>
     <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>20</v>
@@ -857,7 +857,7 @@
     </row>
     <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>21</v>
@@ -865,7 +865,7 @@
     </row>
     <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>22</v>
@@ -873,7 +873,7 @@
     </row>
     <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>23</v>
@@ -881,7 +881,7 @@
     </row>
     <row r="29" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>24</v>
@@ -889,7 +889,7 @@
     </row>
     <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>25</v>
@@ -897,7 +897,7 @@
     </row>
     <row r="31" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>26</v>
@@ -905,7 +905,7 @@
     </row>
     <row r="32" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>27</v>
@@ -913,31 +913,31 @@
     </row>
     <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>16</v>
@@ -945,10 +945,10 @@
     </row>
     <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15" x14ac:dyDescent="0.2">
@@ -966,7 +966,7 @@
         <v>7</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15" x14ac:dyDescent="0.2">
@@ -974,7 +974,7 @@
         <v>7</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15" x14ac:dyDescent="0.2">
@@ -982,7 +982,7 @@
         <v>7</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15" x14ac:dyDescent="0.2">
@@ -992,90 +992,90 @@
     </row>
     <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15" x14ac:dyDescent="0.2">
@@ -1090,31 +1090,31 @@
     </row>
     <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>20</v>
@@ -1122,145 +1122,145 @@
     </row>
     <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Korrekturen von Index und Personenregister
Korrekturen nach der Liste von RH abgearbeitet, die meisten angezeigten Warnungen im Personenregister konnten nicht gelöst werden, da es keine entsprechende GND gibt
</commit_message>
<xml_diff>
--- a/data/xlsx/Baernreither_Index_2023.xlsx
+++ b/data/xlsx/Baernreither_Index_2023.xlsx
@@ -1,20 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28109"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christofaichner/Documents/GitHub/baernreither-data/data/xlsx/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="13725"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13720"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621" refMode="R1C1" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="92">
   <si>
     <t>Bürgertum</t>
   </si>
@@ -283,6 +291,21 @@
   </si>
   <si>
     <t>Versicherung</t>
+  </si>
+  <si>
+    <t>Pressebüro des Ministerratspräsidiums</t>
+  </si>
+  <si>
+    <t>Herrenhaus</t>
+  </si>
+  <si>
+    <t>Allgemeines Wahlrecht</t>
+  </si>
+  <si>
+    <t>Delegationen</t>
+  </si>
+  <si>
+    <t>Realunion</t>
   </si>
 </sst>
 </file>
@@ -351,7 +374,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -655,7 +678,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -663,20 +686,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B83"/>
+  <dimension ref="A1:B90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="32.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.85546875" style="1"/>
+    <col min="1" max="1" width="34.5" style="5" customWidth="1"/>
+    <col min="2" max="2" width="32.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>78</v>
       </c>
@@ -726,7 +749,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>62</v>
       </c>
@@ -734,7 +757,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>62</v>
       </c>
@@ -742,7 +765,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>62</v>
       </c>
@@ -750,7 +773,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>62</v>
       </c>
@@ -758,12 +781,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>66</v>
       </c>
@@ -779,7 +802,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -796,478 +819,528 @@
       <c r="A17" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B17" s="1" t="s">
+    </row>
+    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>3</v>
+        <v>68</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="1" t="s">
+    </row>
+    <row r="24" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+    <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B24" s="1" t="s">
+    </row>
+    <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+    <row r="41" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+    <row r="42" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+    <row r="43" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+    <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+    <row r="45" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+    <row r="46" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+    <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B59" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+    <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+    <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+    <row r="62" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B62" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+    <row r="63" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+      <c r="B63" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B64" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
+    <row r="65" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A65" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
+    <row r="66" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
+    <row r="67" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
+    <row r="68" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
+    <row r="69" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A69" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B69" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
+    <row r="70" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B66" s="1" t="s">
+    <row r="71" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B67" s="1" t="s">
+    <row r="73" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B68" s="1" t="s">
+    <row r="75" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B69" s="1" t="s">
+    <row r="76" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B70" s="1" t="s">
+    <row r="77" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B71" s="1" t="s">
+    <row r="78" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B72" s="1" t="s">
+    <row r="79" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A79" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B73" s="1" t="s">
+    <row r="80" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A80" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B74" s="1" t="s">
+    <row r="81" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A81" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B75" s="1" t="s">
+    <row r="82" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B76" s="1" t="s">
+    <row r="83" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B77" s="1" t="s">
+    <row r="84" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
+    <row r="85" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
+    <row r="86" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A80" s="4"/>
-    </row>
-    <row r="81" spans="1:1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A81" s="2"/>
-    </row>
-    <row r="82" spans="1:1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A82" s="4"/>
-    </row>
-    <row r="83" spans="1:1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A83" s="2"/>
+    <row r="87" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A87" s="4"/>
+    </row>
+    <row r="88" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A88" s="2"/>
+    </row>
+    <row r="89" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A89" s="4"/>
+    </row>
+    <row r="90" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A90" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
test git build data
</commit_message>
<xml_diff>
--- a/data/xlsx/Baernreither_Index_2023.xlsx
+++ b/data/xlsx/Baernreither_Index_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rh\github\baernreither-data\data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D529CB9F-16EB-4074-8A11-22D7410F530C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E466EEF5-4DA2-4137-A665-1FA3A168F342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="2640" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -375,7 +375,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -689,11 +689,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.42578125" style="5" customWidth="1"/>
     <col min="2" max="2" width="32.140625" style="1" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
corrections according to list
</commit_message>
<xml_diff>
--- a/data/xlsx/Baernreither_Index_2023.xlsx
+++ b/data/xlsx/Baernreither_Index_2023.xlsx
@@ -1,22 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christofaichner/Documents/GitHub/baernreither-data/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2715E89D-1A5C-6542-8D98-6DC7249098A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8942E3D-D22A-AC40-9C06-A95546E18D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="MIGAEtrWxjvykv7E4pmlZvogrId1c8BxcQ5Ejh8Kqvs="/>
     </ext>
@@ -1202,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC1034"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>

</xml_diff>